<commit_message>
added capability for the text color font style in HeaderCellStyle DataCellStyle
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/DynamicallyGeneratedExcelProcessorTest.xlsx
+++ b/src/main/resources/excel/DynamicallyGeneratedExcelProcessorTest.xlsx
@@ -88,7 +88,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,7 +112,7 @@
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:sz val="11"/>
-      <main:color theme="1"/>
+      <main:color rgb="FF9C0006"/>
       <main:name val="Calibri"/>
       <main:family val="2"/>
       <main:scheme val="minor"/>
@@ -130,6 +130,30 @@
       <main:name val="Calibri"/>
       <main:family val="2"/>
       <main:scheme val="minor"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="11"/>
+      <main:color theme="1"/>
+      <main:name val="Calibri"/>
+      <main:family val="2"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="23"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="11"/>
+      <main:color theme="1"/>
+      <main:name val="Calibri"/>
+      <main:family val="2"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="23"/>
     </font>
   </fonts>
   <fills count="5">
@@ -190,7 +214,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -200,8 +224,8 @@
       <alignment wrapText="false"/>
       <protection hidden="false"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="1" applyFill="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment horizontal="center" wrapText="false"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="true" applyFill="true" applyNumberFormat="true" applyFont="true">
+      <alignment wrapText="false"/>
       <protection hidden="false"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyBorder="true" applyFill="true" applyNumberFormat="true" applyFont="true">
@@ -212,7 +236,13 @@
       <alignment wrapText="false"/>
       <protection hidden="false"/>
     </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="1" applyFill="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment horizontal="center" wrapText="false"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="1" applyFill="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment horizontal="center" wrapText="false"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
@@ -589,7 +619,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="15.5" hidden="true"/>
-    <col min="2" max="2" customWidth="true" width="15.6640625"/>
+    <col min="2" max="2" customWidth="true" width="15.5"/>
     <col min="3" max="3" customWidth="true" width="15.5"/>
     <col min="4" max="4" customWidth="true" width="15.5"/>
     <col min="5" max="256" customWidth="true" width="8.83203125"/>
@@ -620,7 +650,7 @@
       <c r="A3" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s" s="7">
         <v>13</v>
       </c>
       <c r="C3" t="s" s="0">
@@ -631,11 +661,11 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="7"/>
-      <c r="B4" t="s" s="0">
+      <c r="A4" s="8"/>
+      <c r="B4" t="s" s="9">
         <v>15</v>
       </c>
-      <c r="C4" s="8"/>
+      <c r="C4" s="10"/>
       <c r="D4" t="n" s="0">
         <v>10000.0</v>
       </c>

</xml_diff>